<commit_message>
test_pwm: basic working dma adc timer version
</commit_message>
<xml_diff>
--- a/embedded/test_pwm/DOC/pin分配.xlsx
+++ b/embedded/test_pwm/DOC/pin分配.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t xml:space="preserve"> 序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -120,11 +120,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FSK控制的慢1/4相位,TIM1_CH2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FSK控制,TIM1_CH3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWDIO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWCLK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DIO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FSK控制,TIM1_CH2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>送FSK引脚</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -504,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -572,7 +600,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -589,10 +617,12 @@
         <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" s="4" customFormat="1">
@@ -662,6 +692,40 @@
       <c r="E8" s="3"/>
       <c r="F8" s="5"/>
       <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>